<commit_message>
Modified both ocr files.
</commit_message>
<xml_diff>
--- a/05-simple-ocr-client/output/delivery_notes1.xlsx
+++ b/05-simple-ocr-client/output/delivery_notes1.xlsx
@@ -488,7 +488,8 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>anc suppliers</t>
+          <t>ABC Suppliers Lea
+rotal</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,7 +502,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NEEDS REVIEW</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -537,7 +538,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>NEEDS REVIEW</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -573,7 +574,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>NEEDS REVIEW</t>
+          <t>OK</t>
         </is>
       </c>
     </row>

</xml_diff>